<commit_message>
fixed book request handling
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,6 +477,28 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>8c6976e5b5410415bde908bd4dee15dfb167a9c873fc4bb8a81f6f2ab448a918</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>admin@admin</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>staff</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>